<commit_message>
Turn off electrification for building biomass
</commit_message>
<xml_diff>
--- a/InputData/bldgs/RBFF/Recipient Buildings Fuel Fractions.xlsx
+++ b/InputData/bldgs/RBFF/Recipient Buildings Fuel Fractions.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.5.0-us-wipD\InputData\bldgs\RBFF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-mexico\InputData\bldgs\RBFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4761A941-EE2D-4C0C-A90E-C4D7F53FE0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25815" windowHeight="11295"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RBFF" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -96,7 +107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,19 +440,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -449,42 +460,42 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -496,22 +507,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="6" width="17.28515625" style="5" customWidth="1"/>
-    <col min="7" max="11" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="34.26953125" customWidth="1"/>
+    <col min="2" max="6" width="17.26953125" style="5" customWidth="1"/>
+    <col min="7" max="11" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -546,7 +559,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -566,7 +579,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="5">
         <v>1</v>
@@ -581,7 +594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -616,7 +629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -651,7 +664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -686,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -721,7 +734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -741,7 +754,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="5">
         <v>0</v>
@@ -756,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -791,7 +804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -826,7 +839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -861,7 +874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>

</xml_diff>